<commit_message>
biomass sample randomizations created
</commit_message>
<xml_diff>
--- a/data/2025_PM3D_randomization.xlsx
+++ b/data/2025_PM3D_randomization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\B4I\B4I_hyde\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD7B8A2-8966-426C-A457-C7AC601661CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E2EAA5-7AA9-4F73-8C4C-78F0EEA1A27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{424BB629-4042-4F0E-8B15-D43D67C59135}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="48">
   <si>
     <t>location</t>
   </si>
@@ -80,9 +80,6 @@
     <t>NO_OATS_PLANTED</t>
   </si>
   <si>
-    <t>ND Victory</t>
-  </si>
-  <si>
     <t>mono</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>NDP150412G</t>
   </si>
   <si>
-    <t>ND Dawn</t>
-  </si>
-  <si>
     <t>ND</t>
   </si>
   <si>
@@ -177,13 +171,22 @@
   </si>
   <si>
     <t>20</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>ND DAWN</t>
+  </si>
+  <si>
+    <t>ND VICTORY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +218,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -236,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -253,15 +262,40 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,30 +630,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C865876F-3BB5-4F12-B3EA-947578770ABA}">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="L68" sqref="L68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -644,11 +678,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="13">
         <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -669,21 +703,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="13">
         <v>102</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -694,11 +728,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="13">
         <v>202</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -708,7 +742,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -719,18 +753,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="13">
         <v>201</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
@@ -744,18 +778,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="13">
         <v>301</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -769,21 +803,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="13">
         <v>302</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -794,21 +828,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="13">
         <v>402</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -819,21 +853,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="13">
         <v>401</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -844,18 +878,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="13">
         <v>501</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>12</v>
@@ -869,18 +903,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="13">
         <v>502</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
@@ -894,18 +928,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="13">
         <v>602</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
@@ -919,18 +953,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="13">
         <v>601</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
@@ -944,18 +978,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="13">
         <v>701</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>12</v>
@@ -969,21 +1003,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="13">
         <v>702</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -994,21 +1028,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="13">
         <v>802</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1019,21 +1053,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="13">
         <v>801</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1044,18 +1078,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="13">
         <v>901</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>12</v>
@@ -1069,21 +1103,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="13">
         <v>902</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1094,15 +1128,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="13">
         <v>1002</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>11</v>
@@ -1119,21 +1153,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="13">
         <v>1001</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1144,21 +1178,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1169,18 +1203,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>12</v>
@@ -1194,21 +1228,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1219,18 +1253,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>12</v>
@@ -1244,21 +1278,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1269,18 +1303,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>12</v>
@@ -1294,21 +1328,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1319,15 +1353,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>11</v>
@@ -1344,21 +1378,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1369,15 +1403,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>11</v>
@@ -1394,21 +1428,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -1419,18 +1453,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>12</v>
@@ -1444,21 +1478,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
@@ -1469,18 +1503,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>12</v>
@@ -1494,21 +1528,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -1519,18 +1553,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>12</v>
@@ -1544,21 +1578,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -1569,18 +1603,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>12</v>
@@ -1594,12 +1628,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>13</v>
@@ -1608,7 +1642,7 @@
         <v>11</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -1619,18 +1653,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>12</v>
@@ -1644,21 +1678,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F42" s="4">
         <v>0</v>
@@ -1673,18 +1707,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>12</v>
@@ -1702,21 +1736,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E44" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F44" s="4">
         <v>60</v>
@@ -1731,21 +1765,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F45" s="4">
         <v>60</v>
@@ -1760,18 +1794,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>12</v>
@@ -1789,21 +1823,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F47" s="4">
         <v>0</v>
@@ -1818,18 +1852,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>12</v>
@@ -1847,21 +1881,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F49" s="4">
         <v>0</v>
@@ -1876,21 +1910,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F50" s="4">
         <v>24</v>
@@ -1905,18 +1939,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>12</v>
@@ -1934,21 +1968,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F52" s="4">
         <v>0</v>
@@ -1963,18 +1997,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>12</v>
@@ -1992,12 +2026,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>10</v>
@@ -2021,18 +2055,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>12</v>
@@ -2050,12 +2084,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>13</v>
@@ -2064,7 +2098,7 @@
         <v>11</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F56" s="4">
         <v>0</v>
@@ -2079,21 +2113,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F57" s="4">
         <v>60</v>
@@ -2108,18 +2142,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>12</v>
@@ -2137,15 +2171,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -2166,18 +2200,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>12</v>
@@ -2195,21 +2229,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F61" s="4">
         <v>60</v>
@@ -2224,86 +2258,86 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" s="8">
+        <v>24</v>
+      </c>
+      <c r="B62" s="14">
         <v>401</v>
       </c>
       <c r="C62" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="7">
+        <v>1</v>
+      </c>
+      <c r="I62" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="14">
+        <v>402</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E62" s="6" t="s">
+      <c r="E63" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="7">
+        <v>1</v>
+      </c>
+      <c r="I63" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" s="14">
+        <v>403</v>
+      </c>
+      <c r="C64" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="8">
-        <v>1</v>
-      </c>
-      <c r="I62" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="8">
-        <v>402</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="8">
-        <v>1</v>
-      </c>
-      <c r="I63" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B64" s="8">
-        <v>403</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="D64" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="8">
-        <v>2</v>
-      </c>
-      <c r="I64" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="7">
+        <v>2</v>
+      </c>
+      <c r="I64" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" s="8">
+        <v>24</v>
+      </c>
+      <c r="B65" s="14">
         <v>404</v>
       </c>
       <c r="C65" s="6" t="s">
@@ -2313,147 +2347,147 @@
         <v>11</v>
       </c>
       <c r="E65" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="7">
+        <v>2</v>
+      </c>
+      <c r="I65" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" s="14">
+        <v>405</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="7">
+        <v>3</v>
+      </c>
+      <c r="I66" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" s="14">
+        <v>406</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="7">
+        <v>3</v>
+      </c>
+      <c r="I67" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B68" s="14">
+        <v>407</v>
+      </c>
+      <c r="C68" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F65" s="7"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="8">
-        <v>2</v>
-      </c>
-      <c r="I65" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B66" s="8">
-        <v>405</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="8">
-        <v>3</v>
-      </c>
-      <c r="I66" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="8">
-        <v>406</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="8">
-        <v>3</v>
-      </c>
-      <c r="I67" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="8">
-        <v>407</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="D68" s="6" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="8">
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="7">
         <v>4</v>
       </c>
-      <c r="I68" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I68" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B69" s="8">
+        <v>24</v>
+      </c>
+      <c r="B69" s="14">
         <v>408</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
-      <c r="H69" s="8">
+        <v>14</v>
+      </c>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="7">
         <v>4</v>
       </c>
-      <c r="I69" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I69" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B70" s="8">
+        <v>24</v>
+      </c>
+      <c r="B70" s="14">
         <v>409</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="8">
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="7">
         <v>5</v>
       </c>
-      <c r="I70" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I70" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B71" s="8">
+        <v>24</v>
+      </c>
+      <c r="B71" s="14">
         <v>410</v>
       </c>
       <c r="C71" s="6" t="s">
@@ -2465,74 +2499,74 @@
       <c r="E71" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="8">
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="7">
         <v>5</v>
       </c>
-      <c r="I71" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I71" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B72" s="8">
+        <v>24</v>
+      </c>
+      <c r="B72" s="14">
         <v>411</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="8">
+        <v>14</v>
+      </c>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="7">
         <v>6</v>
       </c>
-      <c r="I72" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I72" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B73" s="8">
+        <v>24</v>
+      </c>
+      <c r="B73" s="14">
         <v>412</v>
       </c>
       <c r="C73" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D73" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="E73" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="8">
+        <v>14</v>
+      </c>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="7">
         <v>6</v>
       </c>
-      <c r="I73" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I73" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="8">
+        <v>24</v>
+      </c>
+      <c r="B74" s="14">
         <v>413</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>11</v>
@@ -2540,193 +2574,696 @@
       <c r="E74" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F74" s="7"/>
-      <c r="G74" s="7"/>
-      <c r="H74" s="8">
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="7">
         <v>7</v>
       </c>
-      <c r="I74" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I74" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="8">
+        <v>24</v>
+      </c>
+      <c r="B75" s="14">
         <v>414</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="8">
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="7">
         <v>7</v>
       </c>
-      <c r="I75" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I75" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B76" s="8">
+        <v>24</v>
+      </c>
+      <c r="B76" s="14">
         <v>415</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F76" s="7"/>
-      <c r="G76" s="7"/>
-      <c r="H76" s="8">
+        <v>14</v>
+      </c>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="7">
         <v>8</v>
       </c>
-      <c r="I76" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I76" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B77" s="8">
+        <v>24</v>
+      </c>
+      <c r="B77" s="14">
         <v>416</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D77" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="7">
+        <v>8</v>
+      </c>
+      <c r="I77" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B78" s="14">
+        <v>417</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E77" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F77" s="7"/>
-      <c r="G77" s="7"/>
-      <c r="H77" s="8">
-        <v>8</v>
-      </c>
-      <c r="I77" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" s="8">
-        <v>417</v>
-      </c>
-      <c r="C78" s="6" t="s">
+      <c r="E78" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="7">
+        <v>9</v>
+      </c>
+      <c r="I78" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B79" s="14">
+        <v>418</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="7">
+        <v>9</v>
+      </c>
+      <c r="I79" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" s="14">
+        <v>419</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D80" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D78" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F78" s="7"/>
-      <c r="G78" s="7"/>
-      <c r="H78" s="8">
-        <v>9</v>
-      </c>
-      <c r="I78" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B79" s="8">
-        <v>418</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F79" s="7"/>
-      <c r="G79" s="7"/>
-      <c r="H79" s="8">
-        <v>9</v>
-      </c>
-      <c r="I79" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B80" s="8">
-        <v>419</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="E80" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F80" s="7"/>
-      <c r="G80" s="7"/>
-      <c r="H80" s="8">
-        <v>10</v>
-      </c>
-      <c r="I80" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="7">
+        <v>10</v>
+      </c>
+      <c r="I80" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B81" s="8">
+        <v>24</v>
+      </c>
+      <c r="B81" s="14">
         <v>420</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E81" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="7">
+        <v>10</v>
+      </c>
+      <c r="I81" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="10">
+        <v>21</v>
+      </c>
+      <c r="I82" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F83" s="8"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="10">
+        <v>20</v>
+      </c>
+      <c r="I83" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="10">
+        <v>19</v>
+      </c>
+      <c r="I84" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="10">
+        <v>18</v>
+      </c>
+      <c r="I85" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="10">
+        <v>17</v>
+      </c>
+      <c r="I86" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" s="8"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="10">
+        <v>16</v>
+      </c>
+      <c r="I87" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="10">
         <v>15</v>
       </c>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7"/>
-      <c r="H81" s="8">
-        <v>10</v>
-      </c>
-      <c r="I81" s="8">
-        <v>2</v>
+      <c r="I88" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B89" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="10">
+        <v>14</v>
+      </c>
+      <c r="I89" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B90" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="10">
+        <v>13</v>
+      </c>
+      <c r="I90" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B91" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" s="8"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="10">
+        <v>12</v>
+      </c>
+      <c r="I91" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="8"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="10">
+        <v>11</v>
+      </c>
+      <c r="I92" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="10">
+        <v>10</v>
+      </c>
+      <c r="I93" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="10">
+        <v>9</v>
+      </c>
+      <c r="I94" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95" s="8"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="10">
+        <v>8</v>
+      </c>
+      <c r="I95" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F96" s="8"/>
+      <c r="G96" s="8"/>
+      <c r="H96" s="10">
+        <v>7</v>
+      </c>
+      <c r="I96" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97" s="8"/>
+      <c r="G97" s="8"/>
+      <c r="H97" s="10">
+        <v>6</v>
+      </c>
+      <c r="I97" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B98" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F98" s="8"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="10">
+        <v>5</v>
+      </c>
+      <c r="I98" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B99" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99" s="8"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="10">
+        <v>4</v>
+      </c>
+      <c r="I99" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B100" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="10">
+        <v>3</v>
+      </c>
+      <c r="I100" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="10">
+        <v>2</v>
+      </c>
+      <c r="I101" s="10">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B82:B101 B22:B61" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>